<commit_message>
Fixed eigenvector calculation, now outputs ranks back
</commit_message>
<xml_diff>
--- a/APPM3310/SECMatrix.xlsx
+++ b/APPM3310/SECMatrix.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APPM3310\APPM3310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C582D1-E55A-4BB9-9F0E-126E1C45EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC61820-E743-475E-970E-E9F740B33F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{87694B22-A654-4FB3-9518-899E98B4D83E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="19" uniqueCount="19">
   <si>
     <t>Alabama</t>
   </si>
@@ -87,13 +87,19 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,12 +124,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,7 +150,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -293,7 +301,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -317,9 +325,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -343,7 +351,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -378,7 +386,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -396,7 +404,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -421,7 +429,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -457,23 +465,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBC8246-A8DB-4803-932C-E00027416AF1}">
-  <dimension ref="A1:R18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBC8246-A8DB-4803-932C-E00027416AF1}">
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="true" zoomScale="96" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="true"/>
+    <col min="9" max="9" width="14.59765625" customWidth="true"/>
+    <col min="13" max="13" width="13.296875" customWidth="true"/>
+    <col min="14" max="14" width="10.59765625" customWidth="true"/>
+    <col min="16" max="16" width="11.5" customWidth="true"/>
+    <col min="2" max="2" width="11.5" customWidth="true"/>
+    <col min="3" max="3" width="11.5" customWidth="true"/>
+    <col min="4" max="4" width="11.5" customWidth="true"/>
+    <col min="5" max="5" width="11.5" customWidth="true"/>
+    <col min="6" max="6" width="11.5" customWidth="true"/>
+    <col min="7" max="7" width="11.5" customWidth="true"/>
+    <col min="8" max="8" width="12.5" customWidth="true"/>
+    <col min="10" max="10" width="11.5" customWidth="true"/>
+    <col min="11" max="11" width="11.5" customWidth="true"/>
+    <col min="12" max="12" width="11.5" customWidth="true"/>
+    <col min="15" max="15" width="11.5" customWidth="true"/>
+    <col min="17" max="17" width="11.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>A2</f>
         <v>Alabama</v>
@@ -542,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -599,7 +619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -656,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -713,7 +733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -770,7 +790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -827,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -884,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -941,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1226,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1340,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1397,7 +1417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1454,9 +1474,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>SUM(B3:B17)</f>
@@ -1521,6 +1541,59 @@
       <c r="Q18">
         <f>SUM(Q2:Q16)</f>
         <v>10</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0">
+        <v>2.7814497437938779</v>
+      </c>
+      <c r="C20" s="0">
+        <v>1.5336218408881446</v>
+      </c>
+      <c r="D20" s="0">
+        <v>3.3339467336773101</v>
+      </c>
+      <c r="E20" s="0">
+        <v>3.0346414030839846</v>
+      </c>
+      <c r="F20" s="0">
+        <v>1.3781296613038059</v>
+      </c>
+      <c r="G20" s="0">
+        <v>2.3011616010231957</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.37819949716345735</v>
+      </c>
+      <c r="I20" s="0">
+        <v>1.315340348708228</v>
+      </c>
+      <c r="J20" s="0">
+        <v>2.0792184606009294</v>
+      </c>
+      <c r="K20" s="0">
+        <v>1.8803254952733148</v>
+      </c>
+      <c r="L20" s="0">
+        <v>1.069561430987569</v>
+      </c>
+      <c r="M20" s="0">
+        <v>0.3474384429159148</v>
+      </c>
+      <c r="N20" s="0">
+        <v>2.5745372104395376</v>
+      </c>
+      <c r="O20" s="0">
+        <v>1.1963116465628461</v>
+      </c>
+      <c r="P20" s="0">
+        <v>1.9904697571292784</v>
+      </c>
+      <c r="Q20" s="0">
+        <v>1.694270628054859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>